<commit_message>
Update the DID efficiency
modified:   did_efficiency.xlsx
</commit_message>
<xml_diff>
--- a/haas/temp/did_efficiency.xlsx
+++ b/haas/temp/did_efficiency.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tcheng8/Downloads/pci-passthrough/haas/temp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{499A9A13-5A4E-A448-8A9D-BEA21BF799B6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D32539F5-DC09-754D-BA64-AE0832C45B1C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="16840" windowHeight="15320" xr2:uid="{7AF5B203-3DCA-7442-8F34-6A1F58C56F38}"/>
+    <workbookView xWindow="7420" yWindow="460" windowWidth="16840" windowHeight="15320" activeTab="1" xr2:uid="{7AF5B203-3DCA-7442-8F34-6A1F58C56F38}"/>
   </bookViews>
   <sheets>
-    <sheet name="did_efficiency" sheetId="1" r:id="rId1"/>
+    <sheet name="summary" sheetId="2" r:id="rId1"/>
+    <sheet name="did_efficiency" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,6 +28,179 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="56">
+  <si>
+    <t>1CPU, 2 iperf threads</t>
+  </si>
+  <si>
+    <t>BANDWIDTH (Mbps)</t>
+  </si>
+  <si>
+    <t>NIC INTERRUPT (Hz)</t>
+  </si>
+  <si>
+    <t>EARLY TIMER INTERRUPT (Hz)</t>
+  </si>
+  <si>
+    <t>LOCAL TIMER INTERRUPT (Hz)</t>
+  </si>
+  <si>
+    <t>WRMSR VM EXIT</t>
+  </si>
+  <si>
+    <t>TIMER INTERRUPT VM EXIT</t>
+  </si>
+  <si>
+    <t>HOST</t>
+  </si>
+  <si>
+    <t>933.99 ± 2.14</t>
+  </si>
+  <si>
+    <t>4607 ± 12</t>
+  </si>
+  <si>
+    <t>353 ± 2</t>
+  </si>
+  <si>
+    <t>GUEST</t>
+  </si>
+  <si>
+    <t>934.33 ± 2.62</t>
+  </si>
+  <si>
+    <t>4634 ± 23</t>
+  </si>
+  <si>
+    <t>354 ± 1</t>
+  </si>
+  <si>
+    <t>GUEST + DTID</t>
+  </si>
+  <si>
+    <t>934.42 ± 2.00</t>
+  </si>
+  <si>
+    <t>4343± 30</t>
+  </si>
+  <si>
+    <t>4339 ± 30</t>
+  </si>
+  <si>
+    <t>352 ± 1</t>
+  </si>
+  <si>
+    <t>INFINIBAND (Gbps)</t>
+  </si>
+  <si>
+    <t>33.43 ± 0.18</t>
+  </si>
+  <si>
+    <t>57663 ± 548</t>
+  </si>
+  <si>
+    <t>354 ± 2</t>
+  </si>
+  <si>
+    <t>35.52 ± 0.20</t>
+  </si>
+  <si>
+    <t>63743 ± 557</t>
+  </si>
+  <si>
+    <t>35.66 ± 0.17</t>
+  </si>
+  <si>
+    <t>54213 ± 347</t>
+  </si>
+  <si>
+    <t>54165 ± 346</t>
+  </si>
+  <si>
+    <t>2CPU, 2 iperf threads</t>
+  </si>
+  <si>
+    <t>CORE</t>
+  </si>
+  <si>
+    <t>37.50 ± 0.12</t>
+  </si>
+  <si>
+    <t>144716 ± 455</t>
+  </si>
+  <si>
+    <t>251 ± 3</t>
+  </si>
+  <si>
+    <t>37.28 ± 0.33</t>
+  </si>
+  <si>
+    <t>349 ± 16</t>
+  </si>
+  <si>
+    <t>123862 ± 1273</t>
+  </si>
+  <si>
+    <t>255 ± 16</t>
+  </si>
+  <si>
+    <t>36.36 ± 1.32</t>
+  </si>
+  <si>
+    <t>1799 ± 165</t>
+  </si>
+  <si>
+    <t>349 ± 17</t>
+  </si>
+  <si>
+    <t>115262 ± 782</t>
+  </si>
+  <si>
+    <t>110880 ± 826</t>
+  </si>
+  <si>
+    <t>255 ± 17</t>
+  </si>
+  <si>
+    <t>EARLY vCPU/pCPU</t>
+  </si>
+  <si>
+    <t>BAREMETAL</t>
+  </si>
+  <si>
+    <t>GUEST: NO DTID</t>
+  </si>
+  <si>
+    <t>GUEST: DTID</t>
+  </si>
+  <si>
+    <t>0 ± 0</t>
+  </si>
+  <si>
+    <t>1 ± 1</t>
+  </si>
+  <si>
+    <t>9 ± 2</t>
+  </si>
+  <si>
+    <t>2 ± 2</t>
+  </si>
+  <si>
+    <t>ONTIME  vCPU/pCPU</t>
+  </si>
+  <si>
+    <t>251 ± 1</t>
+  </si>
+  <si>
+    <t>254 ± 1</t>
+  </si>
+  <si>
+    <t>250 ± 0</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -375,13 +549,519 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F683110F-78B0-0F40-AD2F-E77E0E7072AB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC1344A5-4098-A444-B52B-2C0C8AD766FC}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F683110F-78B0-0F40-AD2F-E77E0E7072AB}">
+  <dimension ref="A1:K30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="21" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3">
+        <v>353</v>
+      </c>
+      <c r="G3">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8">
+        <v>352</v>
+      </c>
+      <c r="G8">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15" t="s">
+        <v>35</v>
+      </c>
+      <c r="G15">
+        <v>1904</v>
+      </c>
+      <c r="H15">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" t="s">
+        <v>40</v>
+      </c>
+      <c r="G17">
+        <v>1414</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <v>3</v>
+      </c>
+      <c r="F21">
+        <v>4</v>
+      </c>
+      <c r="G21">
+        <v>5</v>
+      </c>
+      <c r="H21">
+        <v>6</v>
+      </c>
+      <c r="I21">
+        <v>7</v>
+      </c>
+      <c r="J21">
+        <v>8</v>
+      </c>
+      <c r="K21">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" t="s">
+        <v>49</v>
+      </c>
+      <c r="F24" t="s">
+        <v>50</v>
+      </c>
+      <c r="G24" t="s">
+        <v>49</v>
+      </c>
+      <c r="H24" t="s">
+        <v>49</v>
+      </c>
+      <c r="I24" t="s">
+        <v>51</v>
+      </c>
+      <c r="J24" t="s">
+        <v>48</v>
+      </c>
+      <c r="K24" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="E27">
+        <v>3</v>
+      </c>
+      <c r="F27">
+        <v>4</v>
+      </c>
+      <c r="G27">
+        <v>5</v>
+      </c>
+      <c r="H27">
+        <v>6</v>
+      </c>
+      <c r="I27">
+        <v>7</v>
+      </c>
+      <c r="J27">
+        <v>8</v>
+      </c>
+      <c r="K27">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" t="s">
+        <v>53</v>
+      </c>
+      <c r="D30" t="s">
+        <v>54</v>
+      </c>
+      <c r="E30" t="s">
+        <v>55</v>
+      </c>
+      <c r="F30" t="s">
+        <v>55</v>
+      </c>
+      <c r="G30" t="s">
+        <v>53</v>
+      </c>
+      <c r="H30" t="s">
+        <v>53</v>
+      </c>
+      <c r="I30" t="s">
+        <v>53</v>
+      </c>
+      <c r="J30" t="s">
+        <v>55</v>
+      </c>
+      <c r="K30" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>